<commit_message>
Literacy modified, Quiz04 added
</commit_message>
<xml_diff>
--- a/data/literacy_1802.xlsx
+++ b/data/literacy_1802.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7503\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coop2711/Google 드라이브/Works/Class/Statistics/R.WD/Class_data/class201802/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC67E80-A8E4-8F49-940C-576D611FDD91}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38260" windowHeight="24740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="566">
   <si>
     <t>과목명 : 생활속의통계학-01(005036)</t>
   </si>
@@ -1385,10 +1386,6 @@
     <t>010-4937-1773</t>
   </si>
   <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>010-8076-6766</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1666,42 +1663,6 @@
   </si>
   <si>
     <t>Q25</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무응답</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1832,8 +1793,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2319,27 +2280,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ182"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI156" sqref="AI156"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J109" sqref="J109:AH109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2313,7 @@
       <c r="H1" s="19"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2387,79 +2348,79 @@
         <v>32</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>534</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>535</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" s="11" customFormat="1">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2481,7 +2442,7 @@
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J3" s="14">
         <v>3</v>
@@ -2559,11 +2520,11 @@
         <v>3</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="AJ3"/>
     </row>
-    <row r="4" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" s="11" customFormat="1">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2613,11 +2574,11 @@
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
       <c r="AI4" s="10" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="AJ4"/>
     </row>
-    <row r="5" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="11" customFormat="1">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2639,7 +2600,7 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J5" s="14">
         <v>3</v>
@@ -2717,11 +2678,11 @@
         <v>2</v>
       </c>
       <c r="AI5" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ5"/>
     </row>
-    <row r="6" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" s="11" customFormat="1">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2821,11 +2782,11 @@
         <v>3</v>
       </c>
       <c r="AI6" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ6"/>
     </row>
-    <row r="7" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="11" customFormat="1">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -2837,17 +2798,17 @@
         <v>20173001</v>
       </c>
       <c r="E7" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>454</v>
-      </c>
-      <c r="F7" s="9">
-        <v>2</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>455</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J7" s="14">
         <v>3</v>
@@ -2925,11 +2886,11 @@
         <v>2</v>
       </c>
       <c r="AI7" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ7"/>
     </row>
-    <row r="8" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="11" customFormat="1">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -3029,11 +2990,11 @@
         <v>2</v>
       </c>
       <c r="AI8" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ8"/>
     </row>
-    <row r="9" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" s="11" customFormat="1">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -3133,11 +3094,11 @@
         <v>2</v>
       </c>
       <c r="AI9" s="10" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="AJ9"/>
     </row>
-    <row r="10" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" s="11" customFormat="1">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -3237,11 +3198,11 @@
         <v>2</v>
       </c>
       <c r="AI10" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ10"/>
     </row>
-    <row r="11" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" s="11" customFormat="1">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -3341,11 +3302,11 @@
         <v>2</v>
       </c>
       <c r="AI11" s="10" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="AJ11"/>
     </row>
-    <row r="12" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" s="11" customFormat="1">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -3409,11 +3370,11 @@
       <c r="AG12" s="10"/>
       <c r="AH12" s="10"/>
       <c r="AI12" s="10" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="AJ12"/>
     </row>
-    <row r="13" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" s="11" customFormat="1">
       <c r="A13" s="9">
         <v>11</v>
       </c>
@@ -3513,11 +3474,11 @@
         <v>2</v>
       </c>
       <c r="AI13" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ13"/>
     </row>
-    <row r="14" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" s="11" customFormat="1">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -3617,11 +3578,11 @@
         <v>2</v>
       </c>
       <c r="AI14" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ14"/>
     </row>
-    <row r="15" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" s="11" customFormat="1">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -3633,17 +3594,17 @@
         <v>20155404</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="F15" s="9">
+        <v>4</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>457</v>
-      </c>
-      <c r="F15" s="9">
-        <v>4</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>458</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J15" s="14">
         <v>3</v>
@@ -3721,11 +3682,11 @@
         <v>2</v>
       </c>
       <c r="AI15" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ15"/>
     </row>
-    <row r="16" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" s="11" customFormat="1">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -3737,17 +3698,17 @@
         <v>20173505</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="F16" s="9">
+        <v>2</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>460</v>
-      </c>
-      <c r="F16" s="9">
-        <v>2</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>461</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J16" s="14">
         <v>3</v>
@@ -3825,11 +3786,11 @@
         <v>2</v>
       </c>
       <c r="AI16" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ16"/>
     </row>
-    <row r="17" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" s="11" customFormat="1">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -3879,11 +3840,11 @@
       <c r="AG17" s="10"/>
       <c r="AH17" s="10"/>
       <c r="AI17" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ17"/>
     </row>
-    <row r="18" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" s="11" customFormat="1">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -3983,11 +3944,11 @@
         <v>2</v>
       </c>
       <c r="AI18" s="10" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="AJ18"/>
     </row>
-    <row r="19" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" s="11" customFormat="1">
       <c r="A19" s="9">
         <v>17</v>
       </c>
@@ -4087,11 +4048,11 @@
         <v>2</v>
       </c>
       <c r="AI19" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ19"/>
     </row>
-    <row r="20" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" s="11" customFormat="1">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -4191,11 +4152,11 @@
         <v>2</v>
       </c>
       <c r="AI20" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ20"/>
     </row>
-    <row r="21" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" s="11" customFormat="1">
       <c r="A21" s="9">
         <v>19</v>
       </c>
@@ -4245,11 +4206,11 @@
       <c r="AG21" s="10"/>
       <c r="AH21" s="10"/>
       <c r="AI21" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ21"/>
     </row>
-    <row r="22" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" s="11" customFormat="1">
       <c r="A22" s="9">
         <v>20</v>
       </c>
@@ -4349,11 +4310,11 @@
         <v>2</v>
       </c>
       <c r="AI22" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ22"/>
     </row>
-    <row r="23" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" s="11" customFormat="1">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -4365,17 +4326,17 @@
         <v>20185214</v>
       </c>
       <c r="E23" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>463</v>
-      </c>
-      <c r="F23" s="9">
-        <v>1</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>464</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
@@ -4403,11 +4364,11 @@
       <c r="AG23" s="10"/>
       <c r="AH23" s="10"/>
       <c r="AI23" s="10" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="AJ23"/>
     </row>
-    <row r="24" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" s="11" customFormat="1">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -4457,11 +4418,11 @@
       <c r="AG24" s="10"/>
       <c r="AH24" s="10"/>
       <c r="AI24" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ24"/>
     </row>
-    <row r="25" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" s="11" customFormat="1">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -4561,11 +4522,11 @@
         <v>2</v>
       </c>
       <c r="AI25" s="10" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="AJ25"/>
     </row>
-    <row r="26" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" s="11" customFormat="1">
       <c r="A26" s="9">
         <v>24</v>
       </c>
@@ -4665,11 +4626,11 @@
         <v>4</v>
       </c>
       <c r="AI26" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ26"/>
     </row>
-    <row r="27" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" s="11" customFormat="1">
       <c r="A27" s="9">
         <v>25</v>
       </c>
@@ -4769,11 +4730,11 @@
         <v>2</v>
       </c>
       <c r="AI27" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ27"/>
     </row>
-    <row r="28" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" s="11" customFormat="1">
       <c r="A28" s="9">
         <v>26</v>
       </c>
@@ -4785,17 +4746,17 @@
         <v>20176211</v>
       </c>
       <c r="E28" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F28" s="9">
+        <v>2</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>466</v>
-      </c>
-      <c r="F28" s="9">
-        <v>2</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>467</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J28" s="14">
         <v>3</v>
@@ -4873,11 +4834,11 @@
         <v>2</v>
       </c>
       <c r="AI28" s="10" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="AJ28"/>
     </row>
-    <row r="29" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" s="11" customFormat="1">
       <c r="A29" s="9">
         <v>27</v>
       </c>
@@ -4977,11 +4938,11 @@
         <v>2</v>
       </c>
       <c r="AI29" s="10" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="AJ29"/>
     </row>
-    <row r="30" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" s="11" customFormat="1">
       <c r="A30" s="9">
         <v>28</v>
       </c>
@@ -5079,11 +5040,11 @@
         <v>2</v>
       </c>
       <c r="AI30" s="10" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="AJ30"/>
     </row>
-    <row r="31" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" s="11" customFormat="1">
       <c r="A31" s="9">
         <v>29</v>
       </c>
@@ -5183,11 +5144,11 @@
         <v>4</v>
       </c>
       <c r="AI31" s="10" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="AJ31"/>
     </row>
-    <row r="32" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" s="11" customFormat="1">
       <c r="A32" s="9">
         <v>30</v>
       </c>
@@ -5287,11 +5248,11 @@
         <v>2</v>
       </c>
       <c r="AI32" s="12" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ32"/>
     </row>
-    <row r="33" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" s="11" customFormat="1">
       <c r="A33" s="9">
         <v>31</v>
       </c>
@@ -5391,11 +5352,11 @@
         <v>2</v>
       </c>
       <c r="AI33" s="10" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="AJ33"/>
     </row>
-    <row r="34" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" s="11" customFormat="1">
       <c r="A34" s="9">
         <v>32</v>
       </c>
@@ -5495,11 +5456,11 @@
         <v>2</v>
       </c>
       <c r="AI34" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ34"/>
     </row>
-    <row r="35" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" s="11" customFormat="1">
       <c r="A35" s="9">
         <v>33</v>
       </c>
@@ -5511,17 +5472,17 @@
         <v>20141111</v>
       </c>
       <c r="E35" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="F35" s="9">
+        <v>4</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>469</v>
-      </c>
-      <c r="F35" s="9">
-        <v>4</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>470</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J35" s="14">
         <v>3</v>
@@ -5599,11 +5560,11 @@
         <v>2</v>
       </c>
       <c r="AI35" s="10" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="AJ35"/>
     </row>
-    <row r="36" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" s="11" customFormat="1">
       <c r="A36" s="9">
         <v>34</v>
       </c>
@@ -5703,11 +5664,11 @@
         <v>2</v>
       </c>
       <c r="AI36" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ36"/>
     </row>
-    <row r="37" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" s="11" customFormat="1">
       <c r="A37" s="9">
         <v>35</v>
       </c>
@@ -5807,11 +5768,11 @@
         <v>1</v>
       </c>
       <c r="AI37" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ37"/>
     </row>
-    <row r="38" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" s="11" customFormat="1">
       <c r="A38" s="9">
         <v>36</v>
       </c>
@@ -5911,11 +5872,11 @@
         <v>2</v>
       </c>
       <c r="AI38" s="10" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="AJ38"/>
     </row>
-    <row r="39" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" s="11" customFormat="1">
       <c r="A39" s="9">
         <v>37</v>
       </c>
@@ -6015,11 +5976,11 @@
         <v>2</v>
       </c>
       <c r="AI39" s="10" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="AJ39"/>
     </row>
-    <row r="40" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" s="11" customFormat="1">
       <c r="A40" s="9">
         <v>38</v>
       </c>
@@ -6069,11 +6030,11 @@
       <c r="AG40" s="10"/>
       <c r="AH40" s="10"/>
       <c r="AI40" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ40"/>
     </row>
-    <row r="41" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" s="11" customFormat="1">
       <c r="A41" s="9">
         <v>39</v>
       </c>
@@ -6173,11 +6134,11 @@
         <v>2</v>
       </c>
       <c r="AI41" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ41"/>
     </row>
-    <row r="42" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" s="11" customFormat="1">
       <c r="A42" s="9">
         <v>40</v>
       </c>
@@ -6277,11 +6238,11 @@
         <v>2</v>
       </c>
       <c r="AI42" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ42"/>
     </row>
-    <row r="43" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" s="11" customFormat="1">
       <c r="A43" s="9">
         <v>41</v>
       </c>
@@ -6381,11 +6342,11 @@
         <v>2</v>
       </c>
       <c r="AI43" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ43"/>
     </row>
-    <row r="44" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" s="11" customFormat="1">
       <c r="A44" s="9">
         <v>42</v>
       </c>
@@ -6485,11 +6446,11 @@
         <v>2</v>
       </c>
       <c r="AI44" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ44"/>
     </row>
-    <row r="45" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" s="11" customFormat="1">
       <c r="A45" s="9">
         <v>43</v>
       </c>
@@ -6589,11 +6550,11 @@
         <v>2</v>
       </c>
       <c r="AI45" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ45"/>
     </row>
-    <row r="46" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" s="11" customFormat="1">
       <c r="A46" s="9">
         <v>44</v>
       </c>
@@ -6693,11 +6654,11 @@
         <v>2</v>
       </c>
       <c r="AI46" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ46"/>
     </row>
-    <row r="47" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" s="11" customFormat="1">
       <c r="A47" s="9">
         <v>45</v>
       </c>
@@ -6797,11 +6758,11 @@
         <v>2</v>
       </c>
       <c r="AI47" s="10" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="AJ47"/>
     </row>
-    <row r="48" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" s="11" customFormat="1">
       <c r="A48" s="9">
         <v>46</v>
       </c>
@@ -6851,11 +6812,11 @@
       <c r="AG48" s="10"/>
       <c r="AH48" s="10"/>
       <c r="AI48" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ48"/>
     </row>
-    <row r="49" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" s="11" customFormat="1">
       <c r="A49" s="9">
         <v>47</v>
       </c>
@@ -6955,11 +6916,11 @@
         <v>2</v>
       </c>
       <c r="AI49" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ49"/>
     </row>
-    <row r="50" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" s="11" customFormat="1">
       <c r="A50" s="9">
         <v>48</v>
       </c>
@@ -7059,11 +7020,11 @@
         <v>2</v>
       </c>
       <c r="AI50" s="10" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="AJ50"/>
     </row>
-    <row r="51" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" s="11" customFormat="1">
       <c r="A51" s="9">
         <v>49</v>
       </c>
@@ -7163,11 +7124,11 @@
         <v>2</v>
       </c>
       <c r="AI51" s="10" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="AJ51"/>
     </row>
-    <row r="52" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" s="11" customFormat="1">
       <c r="A52" s="9">
         <v>50</v>
       </c>
@@ -7267,11 +7228,11 @@
         <v>2</v>
       </c>
       <c r="AI52" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ52"/>
     </row>
-    <row r="53" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" s="11" customFormat="1">
       <c r="A53" s="9">
         <v>51</v>
       </c>
@@ -7283,17 +7244,17 @@
         <v>20133306</v>
       </c>
       <c r="E53" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F53" s="9">
+        <v>4</v>
+      </c>
+      <c r="G53" s="9" t="s">
         <v>472</v>
-      </c>
-      <c r="F53" s="9">
-        <v>4</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>473</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J53" s="14">
         <v>3</v>
@@ -7371,11 +7332,11 @@
         <v>2</v>
       </c>
       <c r="AI53" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ53"/>
     </row>
-    <row r="54" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" s="11" customFormat="1">
       <c r="A54" s="9">
         <v>52</v>
       </c>
@@ -7475,33 +7436,33 @@
         <v>2</v>
       </c>
       <c r="AI54" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ54"/>
     </row>
-    <row r="55" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" s="11" customFormat="1">
       <c r="A55" s="9">
         <v>53</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D55" s="9">
         <v>20152533</v>
       </c>
       <c r="E55" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="F55" s="9">
+        <v>3</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>476</v>
-      </c>
-      <c r="F55" s="9">
-        <v>3</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>477</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J55" s="14">
         <v>3</v>
@@ -7579,11 +7540,11 @@
         <v>2</v>
       </c>
       <c r="AI55" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ55"/>
     </row>
-    <row r="56" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" s="11" customFormat="1">
       <c r="A56" s="9">
         <v>54</v>
       </c>
@@ -7683,11 +7644,11 @@
         <v>2</v>
       </c>
       <c r="AI56" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ56"/>
     </row>
-    <row r="57" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" s="11" customFormat="1">
       <c r="A57" s="9">
         <v>55</v>
       </c>
@@ -7787,11 +7748,11 @@
         <v>2</v>
       </c>
       <c r="AI57" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ57"/>
     </row>
-    <row r="58" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" s="11" customFormat="1">
       <c r="A58" s="9">
         <v>56</v>
       </c>
@@ -7803,17 +7764,17 @@
         <v>20143816</v>
       </c>
       <c r="E58" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="F58" s="9">
+        <v>4</v>
+      </c>
+      <c r="G58" s="9" t="s">
         <v>479</v>
-      </c>
-      <c r="F58" s="9">
-        <v>4</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>480</v>
       </c>
       <c r="H58" s="5"/>
       <c r="I58" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J58" s="14">
         <v>3</v>
@@ -7891,11 +7852,11 @@
         <v>3</v>
       </c>
       <c r="AI58" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ58"/>
     </row>
-    <row r="59" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" s="11" customFormat="1">
       <c r="A59" s="9">
         <v>57</v>
       </c>
@@ -7995,11 +7956,11 @@
         <v>2</v>
       </c>
       <c r="AI59" s="10" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="AJ59"/>
     </row>
-    <row r="60" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" s="11" customFormat="1">
       <c r="A60" s="9">
         <v>58</v>
       </c>
@@ -8049,11 +8010,11 @@
       <c r="AG60" s="10"/>
       <c r="AH60" s="10"/>
       <c r="AI60" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ60"/>
     </row>
-    <row r="61" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" s="11" customFormat="1">
       <c r="A61" s="9">
         <v>59</v>
       </c>
@@ -8153,11 +8114,11 @@
         <v>2</v>
       </c>
       <c r="AI61" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ61"/>
     </row>
-    <row r="62" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" s="11" customFormat="1">
       <c r="A62" s="9">
         <v>60</v>
       </c>
@@ -8169,17 +8130,17 @@
         <v>20186233</v>
       </c>
       <c r="E62" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="F62" s="9">
+        <v>1</v>
+      </c>
+      <c r="G62" s="9" t="s">
         <v>482</v>
-      </c>
-      <c r="F62" s="9">
-        <v>1</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>483</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J62" s="14">
         <v>3</v>
@@ -8257,11 +8218,11 @@
         <v>2</v>
       </c>
       <c r="AI62" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ62"/>
     </row>
-    <row r="63" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" s="11" customFormat="1">
       <c r="A63" s="9">
         <v>61</v>
       </c>
@@ -8361,11 +8322,11 @@
         <v>2</v>
       </c>
       <c r="AI63" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ63"/>
     </row>
-    <row r="64" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" s="11" customFormat="1">
       <c r="A64" s="9">
         <v>62</v>
       </c>
@@ -8465,11 +8426,11 @@
         <v>2</v>
       </c>
       <c r="AI64" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ64"/>
     </row>
-    <row r="65" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" s="11" customFormat="1">
       <c r="A65" s="9">
         <v>63</v>
       </c>
@@ -8481,17 +8442,17 @@
         <v>20175412</v>
       </c>
       <c r="E65" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="F65" s="9">
+        <v>1</v>
+      </c>
+      <c r="G65" s="9" t="s">
         <v>485</v>
-      </c>
-      <c r="F65" s="9">
-        <v>1</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>486</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J65" s="14">
         <v>3</v>
@@ -8569,11 +8530,11 @@
         <v>2</v>
       </c>
       <c r="AI65" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ65"/>
     </row>
-    <row r="66" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" s="11" customFormat="1">
       <c r="A66" s="9">
         <v>64</v>
       </c>
@@ -8585,17 +8546,17 @@
         <v>20121613</v>
       </c>
       <c r="E66" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="F66" s="9">
+        <v>4</v>
+      </c>
+      <c r="G66" s="9" t="s">
         <v>488</v>
-      </c>
-      <c r="F66" s="9">
-        <v>4</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>489</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J66" s="14"/>
       <c r="K66" s="14"/>
@@ -8623,11 +8584,11 @@
       <c r="AG66" s="10"/>
       <c r="AH66" s="10"/>
       <c r="AI66" s="10" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="AJ66"/>
     </row>
-    <row r="67" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" s="11" customFormat="1">
       <c r="A67" s="9">
         <v>65</v>
       </c>
@@ -8727,11 +8688,11 @@
         <v>3</v>
       </c>
       <c r="AI67" s="10" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="AJ67"/>
     </row>
-    <row r="68" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" s="11" customFormat="1">
       <c r="A68" s="9">
         <v>66</v>
       </c>
@@ -8831,11 +8792,11 @@
         <v>2</v>
       </c>
       <c r="AI68" s="10" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="AJ68"/>
     </row>
-    <row r="69" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" s="11" customFormat="1">
       <c r="A69" s="9">
         <v>67</v>
       </c>
@@ -8847,17 +8808,17 @@
         <v>20172840</v>
       </c>
       <c r="E69" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="F69" s="9">
+        <v>2</v>
+      </c>
+      <c r="G69" s="9" t="s">
         <v>491</v>
-      </c>
-      <c r="F69" s="9">
-        <v>2</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>492</v>
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J69" s="14"/>
       <c r="K69" s="14"/>
@@ -8885,11 +8846,11 @@
       <c r="AG69" s="10"/>
       <c r="AH69" s="10"/>
       <c r="AI69" s="10" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="AJ69"/>
     </row>
-    <row r="70" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" s="11" customFormat="1">
       <c r="A70" s="9">
         <v>68</v>
       </c>
@@ -8901,17 +8862,17 @@
         <v>20185131</v>
       </c>
       <c r="E70" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="F70" s="9">
+        <v>1</v>
+      </c>
+      <c r="G70" s="9" t="s">
         <v>494</v>
-      </c>
-      <c r="F70" s="9">
-        <v>1</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>495</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J70" s="14">
         <v>3</v>
@@ -8989,11 +8950,11 @@
         <v>2</v>
       </c>
       <c r="AI70" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ70"/>
     </row>
-    <row r="71" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" s="11" customFormat="1">
       <c r="A71" s="9">
         <v>69</v>
       </c>
@@ -9093,11 +9054,11 @@
         <v>2</v>
       </c>
       <c r="AI71" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ71"/>
     </row>
-    <row r="72" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" s="11" customFormat="1">
       <c r="A72" s="9">
         <v>70</v>
       </c>
@@ -9147,11 +9108,11 @@
       <c r="AG72" s="10"/>
       <c r="AH72" s="10"/>
       <c r="AI72" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ72"/>
     </row>
-    <row r="73" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" s="11" customFormat="1">
       <c r="A73" s="9">
         <v>71</v>
       </c>
@@ -9251,11 +9212,11 @@
         <v>2</v>
       </c>
       <c r="AI73" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ73"/>
     </row>
-    <row r="74" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" s="11" customFormat="1">
       <c r="A74" s="9">
         <v>72</v>
       </c>
@@ -9355,11 +9316,11 @@
         <v>2</v>
       </c>
       <c r="AI74" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ74"/>
     </row>
-    <row r="75" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" s="11" customFormat="1">
       <c r="A75" s="9">
         <v>73</v>
       </c>
@@ -9459,11 +9420,11 @@
         <v>2</v>
       </c>
       <c r="AI75" s="10" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="AJ75"/>
     </row>
-    <row r="76" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" s="11" customFormat="1">
       <c r="A76" s="9">
         <v>74</v>
       </c>
@@ -9563,11 +9524,11 @@
         <v>2</v>
       </c>
       <c r="AI76" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ76"/>
     </row>
-    <row r="77" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" s="11" customFormat="1">
       <c r="A77" s="9">
         <v>75</v>
       </c>
@@ -9667,11 +9628,11 @@
         <v>2</v>
       </c>
       <c r="AI77" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ77"/>
     </row>
-    <row r="78" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" s="11" customFormat="1">
       <c r="A78" s="9">
         <v>76</v>
       </c>
@@ -9771,17 +9732,17 @@
         <v>2</v>
       </c>
       <c r="AI78" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ78"/>
     </row>
-    <row r="79" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" s="11" customFormat="1">
       <c r="A79" s="9">
         <v>77</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D79" s="9">
         <v>20152548</v>
@@ -9875,11 +9836,11 @@
         <v>2</v>
       </c>
       <c r="AI79" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ79"/>
     </row>
-    <row r="80" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" s="11" customFormat="1">
       <c r="A80" s="9">
         <v>78</v>
       </c>
@@ -9979,11 +9940,11 @@
         <v>2</v>
       </c>
       <c r="AI80" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ80"/>
     </row>
-    <row r="81" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:36" s="11" customFormat="1">
       <c r="A81" s="9">
         <v>79</v>
       </c>
@@ -10083,11 +10044,11 @@
         <v>2</v>
       </c>
       <c r="AI81" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ81"/>
     </row>
-    <row r="82" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:36" s="11" customFormat="1">
       <c r="A82" s="9">
         <v>80</v>
       </c>
@@ -10137,11 +10098,11 @@
       <c r="AG82" s="10"/>
       <c r="AH82" s="10"/>
       <c r="AI82" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ82"/>
     </row>
-    <row r="83" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:36" s="11" customFormat="1">
       <c r="A83" s="9">
         <v>81</v>
       </c>
@@ -10241,11 +10202,11 @@
         <v>2</v>
       </c>
       <c r="AI83" s="10" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="AJ83"/>
     </row>
-    <row r="84" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:36" s="11" customFormat="1">
       <c r="A84" s="9">
         <v>82</v>
       </c>
@@ -10257,7 +10218,7 @@
         <v>20157076</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F84" s="9">
         <v>4</v>
@@ -10265,7 +10226,7 @@
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
       <c r="I84" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J84" s="14">
         <v>3</v>
@@ -10343,11 +10304,11 @@
         <v>2</v>
       </c>
       <c r="AI84" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ84"/>
     </row>
-    <row r="85" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:36" s="11" customFormat="1">
       <c r="A85" s="9">
         <v>83</v>
       </c>
@@ -10397,11 +10358,11 @@
       <c r="AG85" s="10"/>
       <c r="AH85" s="10"/>
       <c r="AI85" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ85"/>
     </row>
-    <row r="86" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:36" s="11" customFormat="1">
       <c r="A86" s="9">
         <v>84</v>
       </c>
@@ -10451,11 +10412,11 @@
       <c r="AG86" s="10"/>
       <c r="AH86" s="10"/>
       <c r="AI86" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ86"/>
     </row>
-    <row r="87" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:36" s="11" customFormat="1">
       <c r="A87" s="9">
         <v>85</v>
       </c>
@@ -10555,11 +10516,11 @@
         <v>2</v>
       </c>
       <c r="AI87" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ87"/>
     </row>
-    <row r="88" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:36" s="11" customFormat="1">
       <c r="A88" s="9">
         <v>86</v>
       </c>
@@ -10659,11 +10620,11 @@
         <v>2</v>
       </c>
       <c r="AI88" s="10" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="AJ88"/>
     </row>
-    <row r="89" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:36" s="11" customFormat="1">
       <c r="A89" s="9">
         <v>87</v>
       </c>
@@ -10763,11 +10724,11 @@
         <v>2</v>
       </c>
       <c r="AI89" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ89"/>
     </row>
-    <row r="90" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:36" s="11" customFormat="1">
       <c r="A90" s="9">
         <v>88</v>
       </c>
@@ -10867,11 +10828,11 @@
         <v>2</v>
       </c>
       <c r="AI90" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ90"/>
     </row>
-    <row r="91" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:36" s="11" customFormat="1">
       <c r="A91" s="9">
         <v>89</v>
       </c>
@@ -10971,11 +10932,11 @@
         <v>2</v>
       </c>
       <c r="AI91" s="10" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="AJ91"/>
     </row>
-    <row r="92" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:36" s="11" customFormat="1">
       <c r="A92" s="9">
         <v>90</v>
       </c>
@@ -11075,11 +11036,11 @@
         <v>2</v>
       </c>
       <c r="AI92" s="10" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="AJ92"/>
     </row>
-    <row r="93" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:36" s="11" customFormat="1">
       <c r="A93" s="9">
         <v>91</v>
       </c>
@@ -11179,11 +11140,11 @@
         <v>2</v>
       </c>
       <c r="AI93" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ93"/>
     </row>
-    <row r="94" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:36" s="11" customFormat="1">
       <c r="A94" s="9">
         <v>92</v>
       </c>
@@ -11233,11 +11194,11 @@
       <c r="AG94" s="10"/>
       <c r="AH94" s="10"/>
       <c r="AI94" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ94"/>
     </row>
-    <row r="95" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:36" s="11" customFormat="1">
       <c r="A95" s="9">
         <v>93</v>
       </c>
@@ -11337,11 +11298,11 @@
         <v>2</v>
       </c>
       <c r="AI95" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ95"/>
     </row>
-    <row r="96" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:36" s="11" customFormat="1">
       <c r="A96" s="9">
         <v>94</v>
       </c>
@@ -11441,11 +11402,11 @@
         <v>2</v>
       </c>
       <c r="AI96" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ96"/>
     </row>
-    <row r="97" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:36" s="11" customFormat="1">
       <c r="A97" s="9">
         <v>95</v>
       </c>
@@ -11545,11 +11506,11 @@
         <v>2</v>
       </c>
       <c r="AI97" s="10" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="AJ97"/>
     </row>
-    <row r="98" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:36" s="11" customFormat="1">
       <c r="A98" s="9">
         <v>96</v>
       </c>
@@ -11649,11 +11610,11 @@
         <v>2</v>
       </c>
       <c r="AI98" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ98"/>
     </row>
-    <row r="99" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:36" s="11" customFormat="1">
       <c r="A99" s="9">
         <v>97</v>
       </c>
@@ -11753,11 +11714,11 @@
         <v>2</v>
       </c>
       <c r="AI99" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ99"/>
     </row>
-    <row r="100" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:36" s="11" customFormat="1">
       <c r="A100" s="9">
         <v>98</v>
       </c>
@@ -11857,11 +11818,11 @@
         <v>2</v>
       </c>
       <c r="AI100" s="10" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="AJ100"/>
     </row>
-    <row r="101" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:36" s="11" customFormat="1">
       <c r="A101" s="9">
         <v>99</v>
       </c>
@@ -11961,11 +11922,11 @@
         <v>4</v>
       </c>
       <c r="AI101" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ101"/>
     </row>
-    <row r="102" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:36" s="11" customFormat="1">
       <c r="A102" s="9">
         <v>100</v>
       </c>
@@ -12065,11 +12026,11 @@
         <v>2</v>
       </c>
       <c r="AI102" s="10" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
       <c r="AJ102"/>
     </row>
-    <row r="103" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:36" s="11" customFormat="1">
       <c r="A103" s="9">
         <v>101</v>
       </c>
@@ -12169,11 +12130,11 @@
         <v>2</v>
       </c>
       <c r="AI103" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ103"/>
     </row>
-    <row r="104" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:36" s="11" customFormat="1">
       <c r="A104" s="9">
         <v>102</v>
       </c>
@@ -12223,11 +12184,11 @@
       <c r="AG104" s="10"/>
       <c r="AH104" s="10"/>
       <c r="AI104" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ104"/>
     </row>
-    <row r="105" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:36" s="11" customFormat="1">
       <c r="A105" s="9">
         <v>103</v>
       </c>
@@ -12327,11 +12288,11 @@
         <v>2</v>
       </c>
       <c r="AI105" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ105"/>
     </row>
-    <row r="106" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:36" s="11" customFormat="1">
       <c r="A106" s="9">
         <v>104</v>
       </c>
@@ -12431,11 +12392,11 @@
         <v>2</v>
       </c>
       <c r="AI106" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ106"/>
     </row>
-    <row r="107" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:36" s="11" customFormat="1">
       <c r="A107" s="9">
         <v>105</v>
       </c>
@@ -12485,11 +12446,11 @@
       <c r="AG107" s="10"/>
       <c r="AH107" s="10"/>
       <c r="AI107" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ107"/>
     </row>
-    <row r="108" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:36" s="11" customFormat="1">
       <c r="A108" s="9">
         <v>106</v>
       </c>
@@ -12589,11 +12550,11 @@
         <v>2</v>
       </c>
       <c r="AI108" s="10" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="AJ108"/>
     </row>
-    <row r="109" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:36" s="11" customFormat="1">
       <c r="A109" s="9">
         <v>107</v>
       </c>
@@ -12617,87 +12578,37 @@
       <c r="I109" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="J109" s="14" t="s">
-        <v>451</v>
-      </c>
-      <c r="K109" s="14" t="s">
-        <v>536</v>
-      </c>
-      <c r="L109" s="8" t="s">
-        <v>537</v>
-      </c>
-      <c r="M109" s="14" t="s">
-        <v>538</v>
-      </c>
-      <c r="N109" s="10" t="s">
-        <v>539</v>
-      </c>
-      <c r="O109" s="10" t="s">
-        <v>539</v>
-      </c>
-      <c r="P109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="Q109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="R109" s="10" t="s">
-        <v>541</v>
-      </c>
-      <c r="S109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="T109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="U109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="V109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="W109" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="X109" s="10" t="s">
-        <v>537</v>
-      </c>
-      <c r="Y109" s="10" t="s">
-        <v>541</v>
-      </c>
-      <c r="Z109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="AA109" s="10" t="s">
-        <v>543</v>
-      </c>
-      <c r="AB109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="AC109" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="AD109" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="AE109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="AF109" s="10" t="s">
-        <v>537</v>
-      </c>
-      <c r="AG109" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="AH109" s="10" t="s">
-        <v>540</v>
-      </c>
+      <c r="J109" s="14"/>
+      <c r="K109" s="14"/>
+      <c r="L109" s="8"/>
+      <c r="M109" s="14"/>
+      <c r="N109" s="10"/>
+      <c r="O109" s="10"/>
+      <c r="P109" s="10"/>
+      <c r="Q109" s="10"/>
+      <c r="R109" s="10"/>
+      <c r="S109" s="10"/>
+      <c r="T109" s="10"/>
+      <c r="U109" s="10"/>
+      <c r="V109" s="10"/>
+      <c r="W109" s="10"/>
+      <c r="X109" s="10"/>
+      <c r="Y109" s="10"/>
+      <c r="Z109" s="10"/>
+      <c r="AA109" s="10"/>
+      <c r="AB109" s="10"/>
+      <c r="AC109" s="10"/>
+      <c r="AD109" s="10"/>
+      <c r="AE109" s="10"/>
+      <c r="AF109" s="10"/>
+      <c r="AG109" s="10"/>
+      <c r="AH109" s="10"/>
       <c r="AI109" s="10" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="AJ109"/>
     </row>
-    <row r="110" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:36" s="11" customFormat="1">
       <c r="A110" s="9">
         <v>108</v>
       </c>
@@ -12797,11 +12708,11 @@
         <v>2</v>
       </c>
       <c r="AI110" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ110"/>
     </row>
-    <row r="111" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:36" s="11" customFormat="1">
       <c r="A111" s="9">
         <v>109</v>
       </c>
@@ -12901,11 +12812,11 @@
         <v>2</v>
       </c>
       <c r="AI111" s="10" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="AJ111"/>
     </row>
-    <row r="112" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:36" s="11" customFormat="1">
       <c r="A112" s="9">
         <v>110</v>
       </c>
@@ -13005,11 +12916,11 @@
         <v>2</v>
       </c>
       <c r="AI112" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ112"/>
     </row>
-    <row r="113" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:36" s="11" customFormat="1">
       <c r="A113" s="9">
         <v>111</v>
       </c>
@@ -13109,11 +13020,11 @@
         <v>2</v>
       </c>
       <c r="AI113" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ113"/>
     </row>
-    <row r="114" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:36" s="11" customFormat="1">
       <c r="A114" s="9">
         <v>112</v>
       </c>
@@ -13213,11 +13124,11 @@
         <v>2</v>
       </c>
       <c r="AI114" s="10" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="AJ114"/>
     </row>
-    <row r="115" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:36" s="11" customFormat="1">
       <c r="A115" s="9">
         <v>113</v>
       </c>
@@ -13317,11 +13228,11 @@
         <v>2</v>
       </c>
       <c r="AI115" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ115"/>
     </row>
-    <row r="116" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:36" s="11" customFormat="1">
       <c r="A116" s="9">
         <v>114</v>
       </c>
@@ -13421,11 +13332,11 @@
         <v>2</v>
       </c>
       <c r="AI116" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ116"/>
     </row>
-    <row r="117" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:36" s="11" customFormat="1">
       <c r="A117" s="9">
         <v>115</v>
       </c>
@@ -13525,11 +13436,11 @@
         <v>2</v>
       </c>
       <c r="AI117" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ117"/>
     </row>
-    <row r="118" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:36" s="11" customFormat="1">
       <c r="A118" s="9">
         <v>116</v>
       </c>
@@ -13541,17 +13452,17 @@
         <v>20143141</v>
       </c>
       <c r="E118" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="F118" s="9">
+        <v>2</v>
+      </c>
+      <c r="G118" s="9" t="s">
         <v>499</v>
-      </c>
-      <c r="F118" s="9">
-        <v>2</v>
-      </c>
-      <c r="G118" s="9" t="s">
-        <v>500</v>
       </c>
       <c r="H118" s="5"/>
       <c r="I118" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J118" s="14">
         <v>3</v>
@@ -13629,11 +13540,11 @@
         <v>2</v>
       </c>
       <c r="AI118" s="10" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="AJ118"/>
     </row>
-    <row r="119" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:36" s="11" customFormat="1">
       <c r="A119" s="9">
         <v>117</v>
       </c>
@@ -13733,11 +13644,11 @@
         <v>2</v>
       </c>
       <c r="AI119" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ119"/>
     </row>
-    <row r="120" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:36" s="11" customFormat="1">
       <c r="A120" s="9">
         <v>118</v>
       </c>
@@ -13837,17 +13748,17 @@
         <v>2</v>
       </c>
       <c r="AI120" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ120"/>
     </row>
-    <row r="121" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:36" s="11" customFormat="1">
       <c r="A121" s="9">
         <v>119</v>
       </c>
       <c r="B121" s="5"/>
       <c r="C121" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D121" s="9">
         <v>20125251</v>
@@ -13941,11 +13852,11 @@
         <v>2</v>
       </c>
       <c r="AI121" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ121"/>
     </row>
-    <row r="122" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:36" s="11" customFormat="1">
       <c r="A122" s="9">
         <v>120</v>
       </c>
@@ -14045,11 +13956,11 @@
         <v>2</v>
       </c>
       <c r="AI122" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ122"/>
     </row>
-    <row r="123" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:36" s="11" customFormat="1">
       <c r="A123" s="9">
         <v>121</v>
       </c>
@@ -14149,11 +14060,11 @@
         <v>4</v>
       </c>
       <c r="AI123" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ123"/>
     </row>
-    <row r="124" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:36" s="11" customFormat="1">
       <c r="A124" s="9">
         <v>122</v>
       </c>
@@ -14253,11 +14164,11 @@
         <v>3</v>
       </c>
       <c r="AI124" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ124"/>
     </row>
-    <row r="125" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:36" s="11" customFormat="1">
       <c r="A125" s="9">
         <v>123</v>
       </c>
@@ -14357,11 +14268,11 @@
         <v>2</v>
       </c>
       <c r="AI125" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ125"/>
     </row>
-    <row r="126" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:36" s="11" customFormat="1">
       <c r="A126" s="9">
         <v>124</v>
       </c>
@@ -14461,11 +14372,11 @@
         <v>2</v>
       </c>
       <c r="AI126" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ126"/>
     </row>
-    <row r="127" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:36" s="11" customFormat="1">
       <c r="A127" s="9">
         <v>125</v>
       </c>
@@ -14565,11 +14476,11 @@
         <v>2</v>
       </c>
       <c r="AI127" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ127"/>
     </row>
-    <row r="128" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:36" s="11" customFormat="1">
       <c r="A128" s="9">
         <v>126</v>
       </c>
@@ -14669,11 +14580,11 @@
         <v>2</v>
       </c>
       <c r="AI128" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ128"/>
     </row>
-    <row r="129" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:36" s="11" customFormat="1">
       <c r="A129" s="9">
         <v>127</v>
       </c>
@@ -14773,11 +14684,11 @@
         <v>2</v>
       </c>
       <c r="AI129" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ129"/>
     </row>
-    <row r="130" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:36" s="11" customFormat="1">
       <c r="A130" s="9">
         <v>128</v>
       </c>
@@ -14877,11 +14788,11 @@
         <v>2</v>
       </c>
       <c r="AI130" s="10" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="AJ130"/>
     </row>
-    <row r="131" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:36" s="11" customFormat="1">
       <c r="A131" s="9">
         <v>129</v>
       </c>
@@ -14981,11 +14892,11 @@
         <v>2</v>
       </c>
       <c r="AI131" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ131"/>
     </row>
-    <row r="132" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:36" s="11" customFormat="1">
       <c r="A132" s="9">
         <v>130</v>
       </c>
@@ -15085,11 +14996,11 @@
         <v>2</v>
       </c>
       <c r="AI132" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ132"/>
     </row>
-    <row r="133" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:36" s="11" customFormat="1">
       <c r="A133" s="9">
         <v>131</v>
       </c>
@@ -15187,11 +15098,11 @@
         <v>2</v>
       </c>
       <c r="AI133" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ133"/>
     </row>
-    <row r="134" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:36" s="11" customFormat="1">
       <c r="A134" s="9">
         <v>132</v>
       </c>
@@ -15291,11 +15202,11 @@
         <v>2</v>
       </c>
       <c r="AI134" s="10" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="AJ134"/>
     </row>
-    <row r="135" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:36" s="11" customFormat="1">
       <c r="A135" s="9">
         <v>133</v>
       </c>
@@ -15307,17 +15218,17 @@
         <v>20172351</v>
       </c>
       <c r="E135" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="F135" s="9">
+        <v>2</v>
+      </c>
+      <c r="G135" s="9" t="s">
         <v>502</v>
-      </c>
-      <c r="F135" s="9">
-        <v>2</v>
-      </c>
-      <c r="G135" s="9" t="s">
-        <v>503</v>
       </c>
       <c r="H135" s="5"/>
       <c r="I135" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J135" s="14"/>
       <c r="K135" s="14"/>
@@ -15345,11 +15256,11 @@
       <c r="AG135" s="10"/>
       <c r="AH135" s="10"/>
       <c r="AI135" s="10" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="AJ135"/>
     </row>
-    <row r="136" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:36" s="11" customFormat="1">
       <c r="A136" s="9">
         <v>134</v>
       </c>
@@ -15449,11 +15360,11 @@
         <v>2</v>
       </c>
       <c r="AI136" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ136"/>
     </row>
-    <row r="137" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:36" s="11" customFormat="1">
       <c r="A137" s="9">
         <v>135</v>
       </c>
@@ -15503,11 +15414,11 @@
       <c r="AG137" s="10"/>
       <c r="AH137" s="10"/>
       <c r="AI137" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ137"/>
     </row>
-    <row r="138" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:36" s="11" customFormat="1">
       <c r="A138" s="9">
         <v>136</v>
       </c>
@@ -15607,11 +15518,11 @@
         <v>2</v>
       </c>
       <c r="AI138" s="10" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="AJ138"/>
     </row>
-    <row r="139" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:36" s="11" customFormat="1">
       <c r="A139" s="9">
         <v>137</v>
       </c>
@@ -15711,11 +15622,11 @@
         <v>2</v>
       </c>
       <c r="AI139" s="10" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="AJ139"/>
     </row>
-    <row r="140" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:36" s="11" customFormat="1">
       <c r="A140" s="9">
         <v>138</v>
       </c>
@@ -15765,11 +15676,11 @@
       <c r="AG140" s="10"/>
       <c r="AH140" s="10"/>
       <c r="AI140" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ140"/>
     </row>
-    <row r="141" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:36" s="11" customFormat="1">
       <c r="A141" s="9">
         <v>139</v>
       </c>
@@ -15869,11 +15780,11 @@
         <v>2</v>
       </c>
       <c r="AI141" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ141"/>
     </row>
-    <row r="142" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:36" s="11" customFormat="1">
       <c r="A142" s="9">
         <v>140</v>
       </c>
@@ -15973,11 +15884,11 @@
         <v>2</v>
       </c>
       <c r="AI142" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ142"/>
     </row>
-    <row r="143" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:36" s="11" customFormat="1">
       <c r="A143" s="9">
         <v>141</v>
       </c>
@@ -16077,11 +15988,11 @@
         <v>2</v>
       </c>
       <c r="AI143" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ143"/>
     </row>
-    <row r="144" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:36" s="11" customFormat="1">
       <c r="A144" s="9">
         <v>142</v>
       </c>
@@ -16181,11 +16092,11 @@
         <v>2</v>
       </c>
       <c r="AI144" s="10" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="AJ144"/>
     </row>
-    <row r="145" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:36" s="11" customFormat="1">
       <c r="A145" s="9">
         <v>143</v>
       </c>
@@ -16285,11 +16196,11 @@
         <v>2</v>
       </c>
       <c r="AI145" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ145"/>
     </row>
-    <row r="146" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:36" s="11" customFormat="1">
       <c r="A146" s="9">
         <v>144</v>
       </c>
@@ -16389,11 +16300,11 @@
         <v>2</v>
       </c>
       <c r="AI146" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ146"/>
     </row>
-    <row r="147" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:36" s="11" customFormat="1">
       <c r="A147" s="9">
         <v>145</v>
       </c>
@@ -16415,7 +16326,7 @@
       </c>
       <c r="H147" s="5"/>
       <c r="I147" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J147" s="14">
         <v>3</v>
@@ -16493,11 +16404,11 @@
         <v>2</v>
       </c>
       <c r="AI147" s="10" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AJ147"/>
     </row>
-    <row r="148" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:36" s="11" customFormat="1">
       <c r="A148" s="9">
         <v>146</v>
       </c>
@@ -16509,17 +16420,17 @@
         <v>20167099</v>
       </c>
       <c r="E148" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="F148" s="9">
+        <v>3</v>
+      </c>
+      <c r="G148" s="9" t="s">
         <v>506</v>
-      </c>
-      <c r="F148" s="9">
-        <v>3</v>
-      </c>
-      <c r="G148" s="9" t="s">
-        <v>507</v>
       </c>
       <c r="H148" s="5"/>
       <c r="I148" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J148" s="14">
         <v>3</v>
@@ -16597,11 +16508,11 @@
         <v>2</v>
       </c>
       <c r="AI148" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ148"/>
     </row>
-    <row r="149" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:36" s="11" customFormat="1">
       <c r="A149" s="9">
         <v>147</v>
       </c>
@@ -16619,7 +16530,7 @@
         <v>4</v>
       </c>
       <c r="G149" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H149" s="5"/>
       <c r="I149" s="9" t="s">
@@ -16701,11 +16612,11 @@
         <v>2</v>
       </c>
       <c r="AI149" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ149"/>
     </row>
-    <row r="150" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:36" s="11" customFormat="1">
       <c r="A150" s="9">
         <v>148</v>
       </c>
@@ -16805,11 +16716,11 @@
         <v>2</v>
       </c>
       <c r="AI150" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ150"/>
     </row>
-    <row r="151" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:36" s="11" customFormat="1">
       <c r="A151" s="13">
         <v>149</v>
       </c>
@@ -16909,11 +16820,11 @@
         <v>2</v>
       </c>
       <c r="AI151" s="10" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ151"/>
     </row>
-    <row r="152" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:36" s="11" customFormat="1">
       <c r="A152" s="14">
         <v>150</v>
       </c>
@@ -16963,11 +16874,11 @@
       <c r="AG152" s="10"/>
       <c r="AH152" s="10"/>
       <c r="AI152" s="10" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ152"/>
     </row>
-    <row r="153" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:36" s="11" customFormat="1">
       <c r="A153" s="9">
         <v>151</v>
       </c>
@@ -17067,11 +16978,11 @@
         <v>2</v>
       </c>
       <c r="AI153" s="15" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AJ153"/>
     </row>
-    <row r="154" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:36" s="11" customFormat="1">
       <c r="A154" s="9">
         <v>152</v>
       </c>
@@ -17171,11 +17082,11 @@
         <v>2</v>
       </c>
       <c r="AI154" s="12" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="AJ154"/>
     </row>
-    <row r="155" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:36" s="11" customFormat="1">
       <c r="A155" s="9">
         <v>153</v>
       </c>
@@ -17275,11 +17186,11 @@
         <v>2</v>
       </c>
       <c r="AI155" s="12" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ155"/>
     </row>
-    <row r="156" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:36" s="11" customFormat="1">
       <c r="A156" s="13">
         <v>154</v>
       </c>
@@ -17379,11 +17290,11 @@
         <v>2</v>
       </c>
       <c r="AI156" s="12" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AJ156"/>
     </row>
-    <row r="157" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:36" s="11" customFormat="1">
       <c r="A157" s="14">
         <v>155</v>
       </c>
@@ -17483,11 +17394,11 @@
         <v>2</v>
       </c>
       <c r="AI157" s="10" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="AJ157"/>
     </row>
-    <row r="158" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:36" s="11" customFormat="1">
       <c r="A158" s="9">
         <v>156</v>
       </c>
@@ -17499,17 +17410,17 @@
         <v>20101459</v>
       </c>
       <c r="E158" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="F158" s="9">
+        <v>4</v>
+      </c>
+      <c r="G158" s="9" t="s">
         <v>510</v>
-      </c>
-      <c r="F158" s="9">
-        <v>4</v>
-      </c>
-      <c r="G158" s="9" t="s">
-        <v>511</v>
       </c>
       <c r="H158" s="5"/>
       <c r="I158" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J158" s="16"/>
       <c r="K158" s="16"/>
@@ -17537,11 +17448,11 @@
       <c r="AG158" s="15"/>
       <c r="AH158" s="15"/>
       <c r="AI158" s="10" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="AJ158"/>
     </row>
-    <row r="159" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:36" s="11" customFormat="1">
       <c r="A159" s="9">
         <v>157</v>
       </c>
@@ -17580,7 +17491,7 @@
       <c r="AH159" s="10"/>
       <c r="AI159" s="10"/>
     </row>
-    <row r="160" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:36" s="11" customFormat="1">
       <c r="A160" s="9">
         <v>158</v>
       </c>
@@ -17619,7 +17530,7 @@
       <c r="AH160" s="10"/>
       <c r="AI160" s="10"/>
     </row>
-    <row r="161" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:35" s="11" customFormat="1">
       <c r="A161" s="13">
         <v>159</v>
       </c>
@@ -17658,7 +17569,7 @@
       <c r="AH161" s="10"/>
       <c r="AI161" s="10"/>
     </row>
-    <row r="162" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:35" s="11" customFormat="1">
       <c r="A162" s="14">
         <v>160</v>
       </c>
@@ -17697,7 +17608,7 @@
       <c r="AH162" s="10"/>
       <c r="AI162" s="10"/>
     </row>
-    <row r="163" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:35" s="11" customFormat="1">
       <c r="A163" s="9">
         <v>161</v>
       </c>
@@ -17736,7 +17647,7 @@
       <c r="AH163" s="10"/>
       <c r="AI163" s="10"/>
     </row>
-    <row r="164" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:35" s="11" customFormat="1">
       <c r="A164" s="9">
         <v>162</v>
       </c>
@@ -17775,7 +17686,7 @@
       <c r="AH164" s="10"/>
       <c r="AI164" s="10"/>
     </row>
-    <row r="165" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:35" s="11" customFormat="1">
       <c r="A165" s="9">
         <v>163</v>
       </c>
@@ -17814,7 +17725,7 @@
       <c r="AH165" s="10"/>
       <c r="AI165" s="10"/>
     </row>
-    <row r="166" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:35" s="11" customFormat="1">
       <c r="A166" s="13">
         <v>164</v>
       </c>
@@ -17853,7 +17764,7 @@
       <c r="AH166" s="10"/>
       <c r="AI166" s="10"/>
     </row>
-    <row r="167" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:35" s="11" customFormat="1">
       <c r="A167" s="14">
         <v>165</v>
       </c>
@@ -17892,7 +17803,7 @@
       <c r="AH167" s="10"/>
       <c r="AI167" s="10"/>
     </row>
-    <row r="168" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:35" s="11" customFormat="1">
       <c r="A168" s="9">
         <v>166</v>
       </c>
@@ -17931,7 +17842,7 @@
       <c r="AH168" s="10"/>
       <c r="AI168" s="10"/>
     </row>
-    <row r="169" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:35" s="11" customFormat="1">
       <c r="A169" s="9">
         <v>167</v>
       </c>
@@ -17970,7 +17881,7 @@
       <c r="AH169" s="10"/>
       <c r="AI169" s="10"/>
     </row>
-    <row r="170" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:35" s="11" customFormat="1">
       <c r="A170" s="9">
         <v>168</v>
       </c>
@@ -18009,7 +17920,7 @@
       <c r="AH170" s="10"/>
       <c r="AI170" s="10"/>
     </row>
-    <row r="171" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:35" s="11" customFormat="1">
       <c r="A171" s="13">
         <v>169</v>
       </c>
@@ -18048,7 +17959,7 @@
       <c r="AH171" s="10"/>
       <c r="AI171" s="10"/>
     </row>
-    <row r="172" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:35" s="11" customFormat="1">
       <c r="A172" s="14">
         <v>170</v>
       </c>
@@ -18087,7 +17998,7 @@
       <c r="AH172" s="10"/>
       <c r="AI172" s="10"/>
     </row>
-    <row r="173" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:35" s="11" customFormat="1">
       <c r="A173" s="9">
         <v>171</v>
       </c>
@@ -18126,7 +18037,7 @@
       <c r="AH173" s="10"/>
       <c r="AI173" s="10"/>
     </row>
-    <row r="174" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:35" s="11" customFormat="1">
       <c r="A174" s="9">
         <v>172</v>
       </c>
@@ -18165,7 +18076,7 @@
       <c r="AH174" s="10"/>
       <c r="AI174" s="10"/>
     </row>
-    <row r="175" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:35" s="11" customFormat="1">
       <c r="A175" s="9">
         <v>173</v>
       </c>
@@ -18204,7 +18115,7 @@
       <c r="AH175" s="10"/>
       <c r="AI175" s="10"/>
     </row>
-    <row r="176" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:35" s="11" customFormat="1">
       <c r="A176" s="13">
         <v>174</v>
       </c>
@@ -18243,7 +18154,7 @@
       <c r="AH176" s="10"/>
       <c r="AI176" s="10"/>
     </row>
-    <row r="177" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:35" s="11" customFormat="1">
       <c r="A177" s="14">
         <v>175</v>
       </c>
@@ -18282,7 +18193,7 @@
       <c r="AH177" s="10"/>
       <c r="AI177" s="10"/>
     </row>
-    <row r="178" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:35" s="11" customFormat="1">
       <c r="A178" s="9">
         <v>176</v>
       </c>
@@ -18321,7 +18232,7 @@
       <c r="AH178" s="10"/>
       <c r="AI178" s="10"/>
     </row>
-    <row r="179" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:35" s="11" customFormat="1">
       <c r="A179" s="9">
         <v>177</v>
       </c>
@@ -18360,7 +18271,7 @@
       <c r="AH179" s="10"/>
       <c r="AI179" s="10"/>
     </row>
-    <row r="180" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:35" s="11" customFormat="1">
       <c r="A180" s="9">
         <v>178</v>
       </c>
@@ -18399,7 +18310,7 @@
       <c r="AH180" s="10"/>
       <c r="AI180" s="10"/>
     </row>
-    <row r="181" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:35" s="11" customFormat="1">
       <c r="A181" s="13">
         <v>179</v>
       </c>
@@ -18438,7 +18349,7 @@
       <c r="AH181" s="10"/>
       <c r="AI181" s="10"/>
     </row>
-    <row r="182" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:35" s="11" customFormat="1">
       <c r="A182" s="14">
         <v>180</v>
       </c>

</xml_diff>